<commit_message>
adding bulk upload date and size validation
</commit_message>
<xml_diff>
--- a/public/uploads/product_data.xlsx
+++ b/public/uploads/product_data.xlsx
@@ -83,22 +83,22 @@
     <t>Red</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>Gant</t>
   </si>
   <si>
     <t>shirt</t>
   </si>
   <si>
-    <t>Producto1</t>
-  </si>
-  <si>
-    <t>Producto2</t>
-  </si>
-  <si>
-    <t>Producto3</t>
+    <t>S</t>
+  </si>
+  <si>
+    <t>parka1</t>
+  </si>
+  <si>
+    <t>parka2</t>
+  </si>
+  <si>
+    <t>parka3</t>
   </si>
 </sst>
 </file>
@@ -427,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +484,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -517,10 +517,10 @@
         <v>888888</v>
       </c>
       <c r="L2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" t="s">
         <v>21</v>
-      </c>
-      <c r="M2" t="s">
-        <v>19</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -528,7 +528,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
@@ -561,10 +561,10 @@
         <v>999</v>
       </c>
       <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
         <v>21</v>
-      </c>
-      <c r="M3" t="s">
-        <v>19</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -605,10 +605,10 @@
         <v>66666</v>
       </c>
       <c r="L4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" t="s">
         <v>21</v>
-      </c>
-      <c r="M4" t="s">
-        <v>19</v>
       </c>
       <c r="N4">
         <v>1</v>

</xml_diff>

<commit_message>
addin new brand endpoint and Size guides
</commit_message>
<xml_diff>
--- a/public/uploads/product_data.xlsx
+++ b/public/uploads/product_data.xlsx
@@ -89,16 +89,16 @@
     <t>shirt</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>parka1</t>
-  </si>
-  <si>
-    <t>parka2</t>
-  </si>
-  <si>
-    <t>parka3</t>
+    <t>pants1</t>
+  </si>
+  <si>
+    <t>pants2</t>
+  </si>
+  <si>
+    <t>pants3</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +487,7 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -520,7 +520,7 @@
         <v>20</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -531,7 +531,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -564,7 +564,7 @@
         <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -575,7 +575,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -608,7 +608,7 @@
         <v>20</v>
       </c>
       <c r="M4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N4">
         <v>1</v>

</xml_diff>